<commit_message>
Data Driven Test by .xls and .xlsx
</commit_message>
<xml_diff>
--- a/Alibaba/data/testWithXlsxData.xlsx
+++ b/Alibaba/data/testWithXlsxData.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="384" yWindow="84" windowWidth="16260" windowHeight="5856"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -45,17 +45,24 @@
     <t>expectedErrorMessage</t>
   </si>
   <si>
-    <t xml:space="preserve">Your account name or password is incorrect. </t>
+    <t>Your account name or password is incorrect. Help</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,8 +88,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,7 +397,71 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -396,65 +470,12 @@
     <col min="3" max="3" width="38.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
+    <row r="1" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>